<commit_message>
Working on ModifiedInputPrpcessing.py; Time overlap conflict Bug found
- Bug: Time overlap conflicts are not being detected by the solver and student's in my problem instance are being assigned to sections that occur at the same time
</commit_message>
<xml_diff>
--- a/ifs-solver/src/main/resources/input/2020-Sem1-CAES-Wvl-no-extra-requests/Courses.xlsx
+++ b/ifs-solver/src/main/resources/input/2020-Sem1-CAES-Wvl-no-extra-requests/Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha\Documents\CS Honours\COMP700 - HP\student-lab-sectioning\ifs-solver\src\main\resources\input\2020-Sem1-CAES-Wvl-no-extra-requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF1A1EB-4428-4342-81C6-74C7B1DC6BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EA035F-6332-46D6-9108-FCBE28B910C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="60" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
   <si>
     <t>course</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>sessionStartTime</t>
+  </si>
+  <si>
+    <t>BIOL222</t>
   </si>
 </sst>
 </file>
@@ -445,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +651,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -657,16 +660,16 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E9" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F9" s="1">
         <v>0.125</v>
       </c>
       <c r="G9">
-        <v>144</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -677,10 +680,10 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="1">
         <v>0.59027777777777779</v>
@@ -700,13 +703,13 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E11" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F11" s="1">
         <v>0.125</v>
@@ -723,13 +726,13 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F12" s="1">
         <v>0.125</v>
@@ -746,10 +749,10 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="1">
         <v>0.59027777777777779</v>
@@ -769,10 +772,10 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E14" s="1">
         <v>0.59027777777777779</v>
@@ -786,25 +789,25 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E15" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F15" s="1">
         <v>0.125</v>
       </c>
       <c r="G15">
-        <v>192</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -815,33 +818,33 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E16" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F16" s="1">
         <v>0.125</v>
       </c>
       <c r="G16">
-        <v>48</v>
+        <v>192</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E17" s="1">
         <v>0.59027777777777779</v>
@@ -861,10 +864,10 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="1">
         <v>0.59027777777777779</v>
@@ -884,10 +887,10 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E19" s="1">
         <v>0.59027777777777779</v>
@@ -907,10 +910,10 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E20" s="1">
         <v>0.59027777777777779</v>
@@ -924,16 +927,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E21" s="1">
         <v>0.59027777777777779</v>
@@ -942,7 +945,7 @@
         <v>0.125</v>
       </c>
       <c r="G21">
-        <v>250</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -953,10 +956,10 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E22" s="1">
         <v>0.59027777777777779</v>
@@ -970,16 +973,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E23" s="1">
         <v>0.59027777777777779</v>
@@ -988,12 +991,12 @@
         <v>0.125</v>
       </c>
       <c r="G23">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1002,7 +1005,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E24" s="1">
         <v>0.59027777777777779</v>
@@ -1011,7 +1014,7 @@
         <v>0.125</v>
       </c>
       <c r="G24">
-        <v>40</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1022,10 +1025,10 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E25" s="1">
         <v>0.59027777777777779</v>
@@ -1045,10 +1048,10 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E26" s="1">
         <v>0.59027777777777779</v>
@@ -1062,16 +1065,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E27" s="1">
         <v>0.59027777777777779</v>
@@ -1080,7 +1083,7 @@
         <v>0.125</v>
       </c>
       <c r="G27">
-        <v>154</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1091,10 +1094,10 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E28" s="1">
         <v>0.59027777777777779</v>
@@ -1103,30 +1106,30 @@
         <v>0.125</v>
       </c>
       <c r="G28">
-        <v>136</v>
+        <v>154</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F29" s="1">
         <v>0.125</v>
       </c>
       <c r="G29">
-        <v>750</v>
+        <v>136</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1137,19 +1140,19 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F30" s="1">
         <v>0.125</v>
       </c>
       <c r="G30">
-        <v>500</v>
+        <v>750</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1160,10 +1163,10 @@
         <v>1</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E31" s="1">
         <v>0.59027777777777779</v>
@@ -1172,21 +1175,21 @@
         <v>0.125</v>
       </c>
       <c r="G31">
-        <v>250</v>
+        <v>500</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D32" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E32" s="1">
         <v>0.59027777777777779</v>
@@ -1195,12 +1198,12 @@
         <v>0.125</v>
       </c>
       <c r="G32">
-        <v>165</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1209,7 +1212,7 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E33" s="1">
         <v>0.59027777777777779</v>
@@ -1218,7 +1221,7 @@
         <v>0.125</v>
       </c>
       <c r="G33">
-        <v>491</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1229,19 +1232,19 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E34" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F34" s="1">
         <v>0.125</v>
       </c>
       <c r="G34">
-        <v>350</v>
+        <v>491</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1252,47 +1255,47 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E35" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F35" s="1">
         <v>0.125</v>
       </c>
       <c r="G35">
-        <v>491</v>
+        <v>350</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E36" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F36" s="1">
         <v>0.125</v>
       </c>
       <c r="G36">
-        <v>106</v>
+        <v>491</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1304,18 +1307,18 @@
         <v>8</v>
       </c>
       <c r="E37" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F37" s="1">
         <v>0.125</v>
       </c>
       <c r="G37">
-        <v>320</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1324,7 +1327,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E38" s="1">
         <v>0.59027777777777779</v>
@@ -1333,7 +1336,7 @@
         <v>0.125</v>
       </c>
       <c r="G38">
-        <v>270</v>
+        <v>320</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1344,10 +1347,10 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39" s="1">
         <v>0.59027777777777779</v>
@@ -1356,7 +1359,7 @@
         <v>0.125</v>
       </c>
       <c r="G39">
-        <v>320</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1367,13 +1370,13 @@
         <v>1</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E40" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F40" s="1">
         <v>0.125</v>
@@ -1390,13 +1393,13 @@
         <v>1</v>
       </c>
       <c r="C41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D41" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E41" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F41" s="1">
         <v>0.125</v>
@@ -1407,19 +1410,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F42" s="1">
         <v>0.125</v>
@@ -1430,7 +1433,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -1439,16 +1442,16 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E43" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F43" s="1">
         <v>0.125</v>
       </c>
       <c r="G43">
-        <v>491</v>
+        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1459,18 +1462,41 @@
         <v>1</v>
       </c>
       <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0.59027777777777779</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="G44">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
         <v>2</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E45" s="1">
         <v>0.39930555555555558</v>
       </c>
-      <c r="F44" s="1">
-        <v>0.125</v>
-      </c>
-      <c r="G44">
+      <c r="F45" s="1">
+        <v>0.125</v>
+      </c>
+      <c r="G45">
         <v>544</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Running the solver after undoing the changes I made to test the time conflict
</commit_message>
<xml_diff>
--- a/ifs-solver/src/main/resources/input/2020-Sem1-CAES-Wvl-no-extra-requests/Courses.xlsx
+++ b/ifs-solver/src/main/resources/input/2020-Sem1-CAES-Wvl-no-extra-requests/Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\talha\Documents\CS Honours\COMP700 - HP\student-lab-sectioning\ifs-solver\src\main\resources\input\2020-Sem1-CAES-Wvl-no-extra-requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EA035F-6332-46D6-9108-FCBE28B910C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A11A521-F72E-49FD-94C1-18CF44B21EC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="60" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
   <si>
     <t>course</t>
   </si>
@@ -127,9 +127,6 @@
   </si>
   <si>
     <t>sessionStartTime</t>
-  </si>
-  <si>
-    <t>BIOL222</t>
   </si>
 </sst>
 </file>
@@ -448,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +648,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -660,16 +657,16 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F9" s="1">
         <v>0.125</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -680,10 +677,10 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E10" s="1">
         <v>0.59027777777777779</v>
@@ -703,13 +700,13 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F11" s="1">
         <v>0.125</v>
@@ -726,13 +723,13 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F12" s="1">
         <v>0.125</v>
@@ -749,10 +746,10 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E13" s="1">
         <v>0.59027777777777779</v>
@@ -772,10 +769,10 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E14" s="1">
         <v>0.59027777777777779</v>
@@ -789,25 +786,25 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
       <c r="C15">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E15" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F15" s="1">
         <v>0.125</v>
       </c>
       <c r="G15">
-        <v>144</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -818,33 +815,33 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E16" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F16" s="1">
         <v>0.125</v>
       </c>
       <c r="G16">
-        <v>192</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E17" s="1">
         <v>0.59027777777777779</v>
@@ -864,10 +861,10 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E18" s="1">
         <v>0.59027777777777779</v>
@@ -887,10 +884,10 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E19" s="1">
         <v>0.59027777777777779</v>
@@ -910,10 +907,10 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E20" s="1">
         <v>0.59027777777777779</v>
@@ -927,16 +924,16 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E21" s="1">
         <v>0.59027777777777779</v>
@@ -945,7 +942,7 @@
         <v>0.125</v>
       </c>
       <c r="G21">
-        <v>48</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -956,10 +953,10 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E22" s="1">
         <v>0.59027777777777779</v>
@@ -973,16 +970,16 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E23" s="1">
         <v>0.59027777777777779</v>
@@ -991,12 +988,12 @@
         <v>0.125</v>
       </c>
       <c r="G23">
-        <v>250</v>
+        <v>260</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1005,7 +1002,7 @@
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E24" s="1">
         <v>0.59027777777777779</v>
@@ -1014,7 +1011,7 @@
         <v>0.125</v>
       </c>
       <c r="G24">
-        <v>260</v>
+        <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1025,10 +1022,10 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E25" s="1">
         <v>0.59027777777777779</v>
@@ -1048,10 +1045,10 @@
         <v>1</v>
       </c>
       <c r="C26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D26" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E26" s="1">
         <v>0.59027777777777779</v>
@@ -1065,16 +1062,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E27" s="1">
         <v>0.59027777777777779</v>
@@ -1083,7 +1080,7 @@
         <v>0.125</v>
       </c>
       <c r="G27">
-        <v>40</v>
+        <v>154</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1094,10 +1091,10 @@
         <v>1</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E28" s="1">
         <v>0.59027777777777779</v>
@@ -1106,30 +1103,30 @@
         <v>0.125</v>
       </c>
       <c r="G28">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F29" s="1">
         <v>0.125</v>
       </c>
       <c r="G29">
-        <v>136</v>
+        <v>750</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1140,19 +1137,19 @@
         <v>1</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D30" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F30" s="1">
         <v>0.125</v>
       </c>
       <c r="G30">
-        <v>750</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1163,10 +1160,10 @@
         <v>1</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E31" s="1">
         <v>0.59027777777777779</v>
@@ -1175,21 +1172,21 @@
         <v>0.125</v>
       </c>
       <c r="G31">
-        <v>500</v>
+        <v>250</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E32" s="1">
         <v>0.59027777777777779</v>
@@ -1198,12 +1195,12 @@
         <v>0.125</v>
       </c>
       <c r="G32">
-        <v>250</v>
+        <v>165</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -1212,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E33" s="1">
         <v>0.59027777777777779</v>
@@ -1221,7 +1218,7 @@
         <v>0.125</v>
       </c>
       <c r="G33">
-        <v>165</v>
+        <v>491</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1232,19 +1229,19 @@
         <v>1</v>
       </c>
       <c r="C34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E34" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F34" s="1">
         <v>0.125</v>
       </c>
       <c r="G34">
-        <v>491</v>
+        <v>350</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1255,47 +1252,47 @@
         <v>1</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E35" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F35" s="1">
         <v>0.125</v>
       </c>
       <c r="G35">
-        <v>350</v>
+        <v>491</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D36" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F36" s="1">
         <v>0.125</v>
       </c>
       <c r="G36">
-        <v>491</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B37">
         <v>1</v>
@@ -1307,18 +1304,18 @@
         <v>8</v>
       </c>
       <c r="E37" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F37" s="1">
         <v>0.125</v>
       </c>
       <c r="G37">
-        <v>106</v>
+        <v>320</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B38">
         <v>1</v>
@@ -1327,7 +1324,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E38" s="1">
         <v>0.59027777777777779</v>
@@ -1336,7 +1333,7 @@
         <v>0.125</v>
       </c>
       <c r="G38">
-        <v>320</v>
+        <v>270</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1347,10 +1344,10 @@
         <v>1</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E39" s="1">
         <v>0.59027777777777779</v>
@@ -1359,7 +1356,7 @@
         <v>0.125</v>
       </c>
       <c r="G39">
-        <v>270</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -1370,13 +1367,13 @@
         <v>1</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E40" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F40" s="1">
         <v>0.125</v>
@@ -1393,13 +1390,13 @@
         <v>1</v>
       </c>
       <c r="C41">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E41" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F41" s="1">
         <v>0.125</v>
@@ -1410,19 +1407,19 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
       <c r="C42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D42" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F42" s="1">
         <v>0.125</v>
@@ -1433,7 +1430,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -1442,16 +1439,16 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E43" s="1">
-        <v>0.39930555555555558</v>
+        <v>0.59027777777777779</v>
       </c>
       <c r="F43" s="1">
         <v>0.125</v>
       </c>
       <c r="G43">
-        <v>320</v>
+        <v>491</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1462,41 +1459,18 @@
         <v>1</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E44" s="1">
-        <v>0.59027777777777779</v>
+        <v>0.39930555555555558</v>
       </c>
       <c r="F44" s="1">
         <v>0.125</v>
       </c>
       <c r="G44">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45">
-        <v>1</v>
-      </c>
-      <c r="C45">
-        <v>2</v>
-      </c>
-      <c r="D45" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0.39930555555555558</v>
-      </c>
-      <c r="F45" s="1">
-        <v>0.125</v>
-      </c>
-      <c r="G45">
         <v>544</v>
       </c>
     </row>

</xml_diff>